<commit_message>
Finished plots for singlebox
</commit_message>
<xml_diff>
--- a/lab5+6/Lab5_template_2018 (1).xlsx
+++ b/lab5+6/Lab5_template_2018 (1).xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikmuj\OneDrive\Documents\Programming\dataplotting\lab 6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ikmuj\OneDrive\Documents\Programming\dataplotting\lab5+6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA19060F-9F2B-4FF3-94FD-9CA06BBE27A0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A437711-4719-405D-91EA-4E13C53556BD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8070" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t>Boxes Tested</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -60,26 +60,6 @@
   </si>
   <si>
     <t>Frequency (Hz)</t>
-  </si>
-  <si>
-    <r>
-      <t>v</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>in</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> (V)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -90,6 +70,7 @@
         <vertAlign val="subscript"/>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve">in </t>
     </r>
@@ -97,6 +78,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> (mA)</t>
     </r>
@@ -149,6 +131,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>Comment on Phase Measurements.</t>
     </r>
@@ -156,6 +139,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -166,6 +150,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>Comments on Model Predictions.</t>
     </r>
@@ -173,6 +158,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -194,12 +180,6 @@
   </si>
   <si>
     <t>Indicate the data used for the model determination (i.e. f0, |Z|, f1, f2, etc.)</t>
-  </si>
-  <si>
-    <t>Indicate phase range and implication thereof.</t>
-  </si>
-  <si>
-    <t>State phase and implication (inductive, resistive or capacitive)</t>
   </si>
   <si>
     <t>Describe how circuit type was arrived upon based on phase characteristics</t>
@@ -226,6 +206,7 @@
         <vertAlign val="superscript"/>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>rst</t>
     </r>
@@ -234,6 +215,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> Lab:</t>
     </r>
@@ -304,6 +286,8 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
       </rPr>
       <t>W</t>
     </r>
@@ -311,6 +295,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>]</t>
     </r>
@@ -328,6 +313,7 @@
         <vertAlign val="subscript"/>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>test</t>
     </r>
@@ -336,6 +322,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> = 0.9994 k</t>
     </r>
@@ -344,6 +331,8 @@
         <b/>
         <sz val="12"/>
         <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
       </rPr>
       <t>W</t>
     </r>
@@ -358,6 +347,7 @@
         <vertAlign val="subscript"/>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>in</t>
     </r>
@@ -366,6 +356,7 @@
         <b/>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>(pp)= 10 V</t>
     </r>
@@ -380,10 +371,83 @@
     <t>Single Port Box. BB-1P-11</t>
   </si>
   <si>
-    <t xml:space="preserve">The only </t>
-  </si>
-  <si>
     <t>Type II</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>0-85, at a resonant freq, resitance is at min, reactance at max</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(v</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>ch2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> v</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (V)</t>
+    </r>
+  </si>
+  <si>
+    <t>The resistance given by the DMM indicates a small resistance, characteristic of the resitance of a inductor. Because the resistor in this case is in series with a capacitor, that side would become an open circuit, leaving the DMM to read the inductor resitance.</t>
+  </si>
+  <si>
+    <t>The resistance of the resistor in parallel with the inductor given by product over sums would be cole to the resitance of the inductor. Because the DMM read a value close to the posible resitance of the inductor, this is also a possible circuit type for my box.</t>
   </si>
   <si>
     <r>
@@ -393,12 +457,25 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> Both have low equivalent resistances</t>
+      <t xml:space="preserve"> Both have low equivalent resistances and are closed circuits</t>
     </r>
-  </si>
-  <si>
-    <t>Type</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>0, implying resistive impedence</t>
+  </si>
+  <si>
+    <t>85, implying inductive impedence due to positive phase</t>
   </si>
 </sst>
 </file>
@@ -409,7 +486,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -418,14 +495,17 @@
       <b/>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -435,34 +515,41 @@
     <font>
       <sz val="12"/>
       <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <vertAlign val="superscript"/>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="11"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <vertAlign val="subscript"/>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -474,11 +561,14 @@
       <vertAlign val="subscript"/>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -497,6 +587,17 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1651,7 +1752,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1691,20 +1792,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="15"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="15"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1750,7 +1842,6 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1772,29 +1863,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="12"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="6"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="8"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="19"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="18"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="14"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="7"/>
     </xf>
@@ -1880,6 +1955,99 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1931,128 +2099,71 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="74" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="163">
@@ -2539,7 +2650,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -2583,7 +2694,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -2607,8 +2718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D53" activeCellId="1" sqref="A53:A72 D53:D72"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2627,101 +2738,101 @@
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="119" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="120"/>
-      <c r="D2" s="93" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="106">
+        <v>34</v>
+      </c>
+      <c r="B2" s="136" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="137"/>
+      <c r="D2" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="92">
         <v>41958</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="121"/>
-      <c r="C3" s="122"/>
+        <v>35</v>
+      </c>
+      <c r="B3" s="138"/>
+      <c r="C3" s="139"/>
       <c r="D3" s="17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="119" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="119"/>
-      <c r="D4" s="119"/>
-      <c r="E4" s="130"/>
+        <v>57</v>
+      </c>
+      <c r="B4" s="136" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="136"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="147"/>
     </row>
     <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="123" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="124"/>
-      <c r="C5" s="124" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="124"/>
-      <c r="E5" s="125"/>
+      <c r="A5" s="140" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="141"/>
+      <c r="C5" s="141" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="141"/>
+      <c r="E5" s="142"/>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="126" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="127"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="97"/>
+      <c r="B6" s="143" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="144"/>
+      <c r="D6" s="85"/>
+      <c r="E6" s="83"/>
     </row>
     <row r="7" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="170" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="171"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="98"/>
+      <c r="B7" s="150" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="151"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="84"/>
     </row>
     <row r="8" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="107" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="168"/>
-      <c r="C8" s="169"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="98"/>
+      <c r="A8" s="93" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="148"/>
+      <c r="C8" s="149"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="84"/>
     </row>
     <row r="9" spans="1:5" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="108" t="s">
+      <c r="A9" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="128" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="129"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="98"/>
+      <c r="B9" s="145" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="146"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="84"/>
     </row>
     <row r="10" spans="1:5" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
@@ -2733,251 +2844,253 @@
       <c r="E10" s="24"/>
     </row>
     <row r="11" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="92" t="s">
+      <c r="A11" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="114" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="115"/>
-      <c r="D11" s="115"/>
-      <c r="E11" s="116"/>
+      <c r="B11" s="131" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="132"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="133"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="164" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="161" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="162"/>
-      <c r="D12" s="162"/>
-      <c r="E12" s="163"/>
+      <c r="A12" s="112" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="115" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="110"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="111"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="164"/>
-      <c r="B13" s="161"/>
-      <c r="C13" s="162"/>
-      <c r="D13" s="162"/>
-      <c r="E13" s="163"/>
+      <c r="A13" s="112"/>
+      <c r="B13" s="109"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="111"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="164"/>
-      <c r="B14" s="161"/>
-      <c r="C14" s="162"/>
-      <c r="D14" s="162"/>
-      <c r="E14" s="163"/>
+      <c r="A14" s="112"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="110"/>
+      <c r="D14" s="110"/>
+      <c r="E14" s="111"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="164"/>
-      <c r="B15" s="161"/>
-      <c r="C15" s="162"/>
-      <c r="D15" s="162"/>
-      <c r="E15" s="163"/>
+      <c r="A15" s="112"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="110"/>
+      <c r="D15" s="110"/>
+      <c r="E15" s="111"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="164"/>
-      <c r="B16" s="161"/>
-      <c r="C16" s="162"/>
-      <c r="D16" s="162"/>
-      <c r="E16" s="163"/>
+      <c r="A16" s="112"/>
+      <c r="B16" s="109"/>
+      <c r="C16" s="110"/>
+      <c r="D16" s="110"/>
+      <c r="E16" s="111"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="164" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="155"/>
-      <c r="C17" s="156"/>
-      <c r="D17" s="156"/>
-      <c r="E17" s="157"/>
+      <c r="A17" s="112" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="115" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="116"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="117"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="165"/>
-      <c r="B18" s="155"/>
-      <c r="C18" s="156"/>
-      <c r="D18" s="156"/>
-      <c r="E18" s="157"/>
+      <c r="A18" s="113"/>
+      <c r="B18" s="115"/>
+      <c r="C18" s="116"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="117"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="165"/>
-      <c r="B19" s="155"/>
-      <c r="C19" s="156"/>
-      <c r="D19" s="156"/>
-      <c r="E19" s="157"/>
+      <c r="A19" s="113"/>
+      <c r="B19" s="115"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="116"/>
+      <c r="E19" s="117"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="165"/>
-      <c r="B20" s="155"/>
-      <c r="C20" s="156"/>
-      <c r="D20" s="156"/>
-      <c r="E20" s="157"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="116"/>
+      <c r="D20" s="116"/>
+      <c r="E20" s="117"/>
     </row>
     <row r="21" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="166"/>
-      <c r="B21" s="158"/>
-      <c r="C21" s="159"/>
-      <c r="D21" s="159"/>
-      <c r="E21" s="160"/>
+      <c r="A21" s="114"/>
+      <c r="B21" s="118"/>
+      <c r="C21" s="119"/>
+      <c r="D21" s="119"/>
+      <c r="E21" s="120"/>
     </row>
     <row r="22" spans="1:5" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="154" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="117"/>
-      <c r="C22" s="117"/>
-      <c r="D22" s="117"/>
-      <c r="E22" s="118"/>
+      <c r="A22" s="167" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="134"/>
+      <c r="C22" s="134"/>
+      <c r="D22" s="134"/>
+      <c r="E22" s="135"/>
     </row>
     <row r="23" spans="1:5" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="30"/>
-      <c r="B23" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="29"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="164" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="165"/>
+      <c r="D23" s="165"/>
+      <c r="E23" s="166"/>
     </row>
     <row r="24" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24" s="131" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="132"/>
-      <c r="D24" s="132"/>
-      <c r="E24" s="133"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="121" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="122"/>
+      <c r="D24" s="122"/>
+      <c r="E24" s="123"/>
     </row>
     <row r="25" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="31"/>
-      <c r="B25" s="167" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="134"/>
-      <c r="D25" s="134"/>
-      <c r="E25" s="135"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="124" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="125"/>
+      <c r="D25" s="125"/>
+      <c r="E25" s="126"/>
     </row>
     <row r="26" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="8"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="20"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="8"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="20"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="8"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="20"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="8"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="20"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="8"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="20"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="B31" s="82" t="s">
-        <v>49</v>
+      <c r="A31" s="28"/>
+      <c r="B31" s="68" t="s">
+        <v>46</v>
       </c>
       <c r="C31" s="3"/>
-      <c r="D31" s="102"/>
+      <c r="D31" s="88"/>
       <c r="E31" s="20"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="8"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="20"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="8"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="20"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="26"/>
-      <c r="C34" s="103"/>
-      <c r="D34" s="103"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="89"/>
       <c r="E34" s="20"/>
     </row>
     <row r="35" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="31"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="26"/>
-      <c r="C35" s="103"/>
-      <c r="D35" s="103"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="89"/>
       <c r="E35" s="20"/>
     </row>
     <row r="36" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="104"/>
-      <c r="B36" s="77"/>
-      <c r="C36" s="77"/>
-      <c r="D36" s="77"/>
-      <c r="E36" s="77"/>
+      <c r="A36" s="90"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="105"/>
+      <c r="A37" s="91"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="105"/>
-      <c r="B38" s="103"/>
-      <c r="C38" s="103"/>
-      <c r="D38" s="103"/>
+      <c r="A38" s="91"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="89"/>
       <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="105"/>
-      <c r="B39" s="103"/>
-      <c r="C39" s="103"/>
-      <c r="D39" s="103"/>
+      <c r="A39" s="91"/>
+      <c r="B39" s="89"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="89"/>
       <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="105"/>
-      <c r="B40" s="103"/>
-      <c r="C40" s="103"/>
-      <c r="D40" s="103"/>
+      <c r="A40" s="91"/>
+      <c r="B40" s="89"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="89"/>
       <c r="E40" s="3"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="105"/>
+      <c r="A41" s="91"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="105"/>
+      <c r="A42" s="91"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="105"/>
+      <c r="A43" s="91"/>
     </row>
     <row r="44" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44"/>
@@ -3010,714 +3123,714 @@
       <c r="D48"/>
     </row>
     <row r="49" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="32" t="s">
+      <c r="A49" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B49" s="33"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="E49" s="54" t="s">
-        <v>42</v>
+      <c r="B49" s="30"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49" s="48" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="155" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="34"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="52"/>
+      <c r="B50" s="156"/>
+      <c r="C50" s="156"/>
+      <c r="D50" s="156"/>
+      <c r="E50" s="157"/>
     </row>
     <row r="51" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="110" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" s="70" t="s">
-        <v>17</v>
-      </c>
-      <c r="C51" s="69"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="109" t="s">
-        <v>58</v>
+      <c r="A51" s="96" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="62"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="95" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="38" t="s">
+      <c r="A52" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="37" t="s">
+      <c r="B52" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C52" s="43" t="s">
+      <c r="D52" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D52" s="46" t="s">
+      <c r="E52" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="E52" s="49" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="53" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="39">
+      <c r="A53" s="34">
         <v>10</v>
       </c>
-      <c r="B53" s="41">
+      <c r="B53" s="36">
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="C53" s="111">
+      <c r="C53" s="97">
         <f>9.8/0.9994</f>
         <v>9.8058835301180718</v>
       </c>
-      <c r="D53" s="47">
+      <c r="D53" s="42">
         <f>B53/(C53*10^-3)</f>
         <v>2.6106775510204079</v>
       </c>
-      <c r="E53" s="50">
+      <c r="E53" s="45">
         <f>(0)*A53*360</f>
         <v>0</v>
       </c>
-      <c r="F53" s="113"/>
+      <c r="F53" s="99"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="40">
+      <c r="A54" s="35">
         <v>20</v>
       </c>
-      <c r="B54" s="42">
+      <c r="B54" s="37">
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="C54" s="112">
+      <c r="C54" s="98">
         <f>9.8/0.9994</f>
         <v>9.8058835301180718</v>
       </c>
-      <c r="D54" s="48">
+      <c r="D54" s="43">
         <f>B54/(C54*10^-3)</f>
         <v>2.6106775510204079</v>
       </c>
-      <c r="E54" s="51">
+      <c r="E54" s="46">
         <f>(0)*A54*360</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="40">
+      <c r="A55" s="35">
         <v>40</v>
       </c>
-      <c r="B55" s="42">
+      <c r="B55" s="37">
         <v>2.64E-2</v>
       </c>
-      <c r="C55" s="45">
+      <c r="C55" s="40">
         <f t="shared" ref="C55:C62" si="0">9.68/0.9994</f>
         <v>9.6858114868921348</v>
       </c>
-      <c r="D55" s="48">
+      <c r="D55" s="43">
         <f t="shared" ref="D55:D72" si="1">B55/(C55*10^-3)</f>
         <v>2.7256363636363639</v>
       </c>
-      <c r="E55" s="51">
+      <c r="E55" s="46">
         <f>(300*10^-6)*A55*360</f>
         <v>4.3199999999999994</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="40">
+      <c r="A56" s="35">
         <v>80</v>
       </c>
-      <c r="B56" s="42">
+      <c r="B56" s="37">
         <v>2.64E-2</v>
       </c>
-      <c r="C56" s="44">
+      <c r="C56" s="39">
         <f t="shared" si="0"/>
         <v>9.6858114868921348</v>
       </c>
-      <c r="D56" s="48">
+      <c r="D56" s="43">
         <f t="shared" si="1"/>
         <v>2.7256363636363639</v>
       </c>
-      <c r="E56" s="51">
+      <c r="E56" s="46">
         <f>(480*10^-6)*A56*360</f>
         <v>13.823999999999998</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="40">
+      <c r="A57" s="35">
         <v>100</v>
       </c>
-      <c r="B57" s="42">
+      <c r="B57" s="37">
         <v>2.7199999999999998E-2</v>
       </c>
-      <c r="C57" s="44">
+      <c r="C57" s="39">
         <f t="shared" si="0"/>
         <v>9.6858114868921348</v>
       </c>
-      <c r="D57" s="48">
+      <c r="D57" s="43">
         <f t="shared" si="1"/>
         <v>2.8082314049586774</v>
       </c>
-      <c r="E57" s="51">
+      <c r="E57" s="46">
         <f>(440*10^-6)*A57*360</f>
         <v>15.84</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="40">
+      <c r="A58" s="35">
         <v>200</v>
       </c>
-      <c r="B58" s="42">
+      <c r="B58" s="37">
         <v>3.04E-2</v>
       </c>
-      <c r="C58" s="44">
+      <c r="C58" s="39">
         <f t="shared" si="0"/>
         <v>9.6858114868921348</v>
       </c>
-      <c r="D58" s="48">
+      <c r="D58" s="43">
         <f t="shared" si="1"/>
         <v>3.1386115702479338</v>
       </c>
-      <c r="E58" s="51">
+      <c r="E58" s="46">
         <f>(420*10^-6)*A58*360</f>
         <v>30.24</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="40">
+      <c r="A59" s="35">
         <v>400</v>
       </c>
-      <c r="B59" s="42">
+      <c r="B59" s="37">
         <v>4.0800000000000003E-2</v>
       </c>
-      <c r="C59" s="112">
+      <c r="C59" s="98">
         <f t="shared" si="0"/>
         <v>9.6858114868921348</v>
       </c>
-      <c r="D59" s="48">
+      <c r="D59" s="43">
         <f t="shared" si="1"/>
         <v>4.212347107438017</v>
       </c>
-      <c r="E59" s="51">
+      <c r="E59" s="46">
         <f>(370*10^-6)*A59*360</f>
         <v>53.279999999999994</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="40">
+      <c r="A60" s="35">
         <v>800</v>
       </c>
-      <c r="B60" s="42">
+      <c r="B60" s="37">
         <v>6.4799999999999996E-2</v>
       </c>
-      <c r="C60" s="112">
+      <c r="C60" s="98">
         <f t="shared" si="0"/>
         <v>9.6858114868921348</v>
       </c>
-      <c r="D60" s="48">
+      <c r="D60" s="43">
         <f t="shared" si="1"/>
         <v>6.6901983471074375</v>
       </c>
-      <c r="E60" s="51">
+      <c r="E60" s="46">
         <f>(240*10^-6)*A60*360</f>
         <v>69.11999999999999</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="40">
+      <c r="A61" s="35">
         <v>1000</v>
       </c>
-      <c r="B61" s="42">
+      <c r="B61" s="37">
         <v>7.9200000000000007E-2</v>
       </c>
-      <c r="C61" s="44">
+      <c r="C61" s="39">
         <f t="shared" si="0"/>
         <v>9.6858114868921348</v>
       </c>
-      <c r="D61" s="48">
+      <c r="D61" s="43">
         <f t="shared" si="1"/>
         <v>8.176909090909092</v>
       </c>
-      <c r="E61" s="51">
+      <c r="E61" s="46">
         <f>(210*10^-6)*A61*360</f>
         <v>75.599999999999994</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="40">
+      <c r="A62" s="35">
         <v>2000</v>
       </c>
-      <c r="B62" s="42">
+      <c r="B62" s="37">
         <v>0.152</v>
       </c>
-      <c r="C62" s="112">
+      <c r="C62" s="98">
         <f t="shared" si="0"/>
         <v>9.6858114868921348</v>
       </c>
-      <c r="D62" s="48">
+      <c r="D62" s="43">
         <f t="shared" si="1"/>
         <v>15.69305785123967</v>
       </c>
-      <c r="E62" s="51">
+      <c r="E62" s="46">
         <f>(118*10^-6)*A62*360</f>
         <v>84.96</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="40">
+      <c r="A63" s="35">
         <v>4000</v>
       </c>
-      <c r="B63" s="42">
+      <c r="B63" s="37">
         <v>0.29399999999999998</v>
       </c>
-      <c r="C63" s="112">
+      <c r="C63" s="98">
         <f>9.76/0.9994</f>
         <v>9.7658595157094261</v>
       </c>
-      <c r="D63" s="48">
+      <c r="D63" s="43">
         <f t="shared" si="1"/>
         <v>30.104877049180324</v>
       </c>
-      <c r="E63" s="51">
+      <c r="E63" s="46">
         <f>(57*10^-6)*A63*360</f>
         <v>82.08</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="40">
+      <c r="A64" s="35">
         <v>8000</v>
       </c>
-      <c r="B64" s="42">
+      <c r="B64" s="37">
         <v>0.58399999999999996</v>
       </c>
-      <c r="C64" s="44">
+      <c r="C64" s="39">
         <f>9.8/0.9994</f>
         <v>9.8058835301180718</v>
       </c>
-      <c r="D64" s="48">
+      <c r="D64" s="43">
         <f t="shared" si="1"/>
         <v>59.556081632653047</v>
       </c>
-      <c r="E64" s="51">
+      <c r="E64" s="46">
         <f>(28.8*10^-6)*A64*360</f>
         <v>82.944000000000003</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="40">
+      <c r="A65" s="35">
         <v>10000</v>
       </c>
-      <c r="B65" s="42">
+      <c r="B65" s="37">
         <v>0.72</v>
       </c>
-      <c r="C65" s="44">
+      <c r="C65" s="39">
         <f>9.8/0.9994</f>
         <v>9.8058835301180718</v>
       </c>
-      <c r="D65" s="48">
+      <c r="D65" s="43">
         <f t="shared" si="1"/>
         <v>73.425306122448973</v>
       </c>
-      <c r="E65" s="51">
+      <c r="E65" s="46">
         <f>(22.4*10^-6)*A65*360</f>
         <v>80.639999999999986</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="40">
+      <c r="A66" s="35">
         <v>20000</v>
       </c>
-      <c r="B66" s="42">
+      <c r="B66" s="37">
         <v>1.4</v>
       </c>
-      <c r="C66" s="44">
+      <c r="C66" s="39">
         <f>9.4/0.9994</f>
         <v>9.4056433860316204</v>
       </c>
-      <c r="D66" s="48">
+      <c r="D66" s="43">
         <f t="shared" si="1"/>
         <v>148.84680851063828</v>
       </c>
-      <c r="E66" s="51">
+      <c r="E66" s="46">
         <f>(10.8*10^-6)*A66*360</f>
         <v>77.760000000000005</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="40">
+      <c r="A67" s="35">
         <v>40000</v>
       </c>
-      <c r="B67" s="42">
+      <c r="B67" s="37">
         <v>2.56</v>
       </c>
-      <c r="C67" s="44">
+      <c r="C67" s="39">
         <f>9/0.9994</f>
         <v>9.0054032419451673</v>
       </c>
-      <c r="D67" s="48">
+      <c r="D67" s="43">
         <f t="shared" si="1"/>
         <v>284.27377777777775</v>
       </c>
-      <c r="E67" s="51">
+      <c r="E67" s="46">
         <f>(5.3*10^-6)*A67*360</f>
         <v>76.319999999999993</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="40">
+      <c r="A68" s="35">
         <v>80000</v>
       </c>
-      <c r="B68" s="42">
+      <c r="B68" s="37">
         <v>3.76</v>
       </c>
-      <c r="C68" s="44">
+      <c r="C68" s="39">
         <f>7.4/0.9994</f>
         <v>7.40444266559936</v>
       </c>
-      <c r="D68" s="48">
+      <c r="D68" s="43">
         <f t="shared" si="1"/>
         <v>507.80324324324317</v>
       </c>
-      <c r="E68" s="51">
+      <c r="E68" s="46">
         <f>(2.08*10^-6)*A68*360</f>
         <v>59.903999999999996</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="40">
+      <c r="A69" s="35">
         <v>100000</v>
       </c>
-      <c r="B69" s="42">
+      <c r="B69" s="37">
         <v>4</v>
       </c>
-      <c r="C69" s="44">
+      <c r="C69" s="39">
         <f>7/0.9994</f>
         <v>7.0042025215129078</v>
       </c>
-      <c r="D69" s="48">
+      <c r="D69" s="43">
         <f t="shared" si="1"/>
         <v>571.08571428571429</v>
       </c>
-      <c r="E69" s="51">
+      <c r="E69" s="46">
         <f>(1.48*10^-6)*A69*360</f>
         <v>53.279999999999994</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="40">
+      <c r="A70" s="35">
         <v>200000</v>
       </c>
-      <c r="B70" s="42">
+      <c r="B70" s="37">
         <v>4.6399999999999997</v>
       </c>
-      <c r="C70" s="44">
+      <c r="C70" s="39">
         <f>5.6/0.9994</f>
         <v>5.6033620172103262</v>
       </c>
-      <c r="D70" s="48">
+      <c r="D70" s="43">
         <f t="shared" si="1"/>
         <v>828.07428571428557</v>
       </c>
-      <c r="E70" s="51">
+      <c r="E70" s="46">
         <f>(480*10^-9)*A70*360</f>
         <v>34.56</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="85">
+      <c r="A71" s="71">
         <v>500000</v>
       </c>
-      <c r="B71" s="86">
+      <c r="B71" s="72">
         <v>4.8</v>
       </c>
-      <c r="C71" s="87">
+      <c r="C71" s="73">
         <f>5/0.9994</f>
         <v>5.0030018010806483</v>
       </c>
-      <c r="D71" s="48">
+      <c r="D71" s="43">
         <f t="shared" si="1"/>
         <v>959.42400000000009</v>
       </c>
-      <c r="E71" s="51">
+      <c r="E71" s="46">
         <f>(56*10^-9)*A71*360</f>
         <v>10.080000000000002</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="88">
+      <c r="A72" s="74">
         <v>750000</v>
       </c>
-      <c r="B72" s="89">
+      <c r="B72" s="75">
         <v>4.76</v>
       </c>
-      <c r="C72" s="90">
+      <c r="C72" s="76">
         <f>4.96/0.9994</f>
         <v>4.9629777866720035</v>
       </c>
-      <c r="D72" s="48">
+      <c r="D72" s="43">
         <f t="shared" si="1"/>
         <v>959.1016129032256</v>
       </c>
-      <c r="E72" s="51">
+      <c r="E72" s="46">
         <f>(12*10^-9)*A72*360</f>
         <v>3.24</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="68" t="s">
-        <v>16</v>
-      </c>
-      <c r="B73" s="66"/>
-      <c r="C73" s="66"/>
-      <c r="D73" s="66"/>
-      <c r="E73" s="67"/>
+      <c r="A73" s="155" t="s">
+        <v>15</v>
+      </c>
+      <c r="B73" s="156"/>
+      <c r="C73" s="156"/>
+      <c r="D73" s="156"/>
+      <c r="E73" s="157"/>
     </row>
     <row r="74" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="61"/>
+      <c r="A74" s="55"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
       <c r="E74" s="7"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="61"/>
+      <c r="A75" s="55"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
       <c r="E75" s="7"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="61"/>
+      <c r="A76" s="55"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
       <c r="E76" s="7"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="61"/>
+      <c r="A77" s="55"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
       <c r="E77" s="7"/>
     </row>
     <row r="78" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="61"/>
+      <c r="A78" s="55"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="7"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="61"/>
+      <c r="A79" s="55"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
       <c r="E79" s="7"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="61"/>
+      <c r="A80" s="55"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
       <c r="E80" s="7"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="61"/>
-      <c r="B81" s="80" t="s">
-        <v>30</v>
+      <c r="A81" s="55"/>
+      <c r="B81" s="66" t="s">
+        <v>29</v>
       </c>
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
       <c r="E81" s="7"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="61"/>
-      <c r="B82" s="80" t="s">
-        <v>28</v>
+      <c r="A82" s="55"/>
+      <c r="B82" s="66" t="s">
+        <v>27</v>
       </c>
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
       <c r="E82" s="7"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="61"/>
-      <c r="B83" s="80" t="s">
-        <v>29</v>
+      <c r="A83" s="55"/>
+      <c r="B83" s="66" t="s">
+        <v>28</v>
       </c>
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
       <c r="E83" s="7"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="61"/>
-      <c r="B84" s="84" t="s">
-        <v>31</v>
+      <c r="A84" s="55"/>
+      <c r="B84" s="70" t="s">
+        <v>30</v>
       </c>
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
       <c r="E84" s="7"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="61"/>
+      <c r="A85" s="55"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
       <c r="E85" s="7"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="61"/>
+      <c r="A86" s="55"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
       <c r="E86" s="7"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="61"/>
+      <c r="A87" s="55"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
       <c r="D87" s="6"/>
       <c r="E87" s="7"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="61"/>
+      <c r="A88" s="55"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
       <c r="E88" s="7"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="61"/>
+      <c r="A89" s="55"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
       <c r="E89" s="7"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="61"/>
+      <c r="A90" s="55"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
       <c r="E90" s="7"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="61"/>
+      <c r="A91" s="55"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
       <c r="E91" s="7"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="61"/>
+      <c r="A92" s="55"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
       <c r="E92" s="7"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="61"/>
+      <c r="A93" s="55"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
       <c r="E93" s="7"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="61"/>
+      <c r="A94" s="55"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
       <c r="E94" s="7"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="61"/>
+      <c r="A95" s="55"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
       <c r="E95" s="7"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="61"/>
+      <c r="A96" s="55"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
       <c r="E96" s="7"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="61"/>
+      <c r="A97" s="55"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
       <c r="D97" s="6"/>
       <c r="E97" s="7"/>
     </row>
     <row r="98" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="62"/>
-      <c r="B98" s="63"/>
-      <c r="C98" s="63"/>
-      <c r="D98" s="63"/>
-      <c r="E98" s="64"/>
+      <c r="A98" s="56"/>
+      <c r="B98" s="57"/>
+      <c r="C98" s="57"/>
+      <c r="D98" s="57"/>
+      <c r="E98" s="58"/>
       <c r="F98"/>
     </row>
     <row r="99" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="32" t="s">
+      <c r="A99" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B99" s="33"/>
-      <c r="C99" s="33"/>
-      <c r="D99" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="E99" s="54" t="s">
-        <v>42</v>
+      <c r="B99" s="30"/>
+      <c r="C99" s="30"/>
+      <c r="D99" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="E99" s="48" t="s">
+        <v>39</v>
       </c>
       <c r="F99"/>
     </row>
     <row r="100" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="65" t="s">
-        <v>12</v>
-      </c>
-      <c r="B100" s="66"/>
-      <c r="C100" s="66"/>
-      <c r="D100" s="66"/>
-      <c r="E100" s="67"/>
+      <c r="A100" s="155" t="s">
+        <v>11</v>
+      </c>
+      <c r="B100" s="156"/>
+      <c r="C100" s="156"/>
+      <c r="D100" s="156"/>
+      <c r="E100" s="157"/>
       <c r="F100"/>
     </row>
     <row r="101" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="55" t="s">
+      <c r="A101" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B101" s="52"/>
+      <c r="C101" s="152" t="s">
+        <v>66</v>
+      </c>
+      <c r="D101" s="153"/>
+      <c r="E101" s="154"/>
+      <c r="F101"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="B101" s="58"/>
-      <c r="C101" s="136" t="s">
-        <v>32</v>
-      </c>
-      <c r="D101" s="137"/>
-      <c r="E101" s="138"/>
-      <c r="F101"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="56" t="s">
+      <c r="B102" s="53"/>
+      <c r="C102" s="168" t="s">
+        <v>72</v>
+      </c>
+      <c r="D102" s="127"/>
+      <c r="E102" s="128"/>
+      <c r="F102"/>
+    </row>
+    <row r="103" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="B102" s="59"/>
-      <c r="C102" s="139" t="s">
-        <v>33</v>
-      </c>
-      <c r="D102" s="140"/>
-      <c r="E102" s="141"/>
-      <c r="F102"/>
-    </row>
-    <row r="103" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="B103" s="60"/>
-      <c r="C103" s="142" t="s">
-        <v>33</v>
-      </c>
-      <c r="D103" s="143"/>
-      <c r="E103" s="144"/>
+      <c r="B103" s="54"/>
+      <c r="C103" s="169" t="s">
+        <v>71</v>
+      </c>
+      <c r="D103" s="129"/>
+      <c r="E103" s="130"/>
       <c r="F103"/>
     </row>
     <row r="104" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="91" t="s">
-        <v>34</v>
+      <c r="A104" s="77" t="s">
+        <v>31</v>
       </c>
       <c r="B104" s="11"/>
       <c r="C104" s="11"/>
@@ -3742,17 +3855,17 @@
       <c r="F106"/>
     </row>
     <row r="107" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="65" t="s">
-        <v>14</v>
-      </c>
-      <c r="B107" s="66"/>
-      <c r="C107" s="66"/>
-      <c r="D107" s="66"/>
-      <c r="E107" s="67"/>
+      <c r="A107" s="155" t="s">
+        <v>13</v>
+      </c>
+      <c r="B107" s="156"/>
+      <c r="C107" s="156"/>
+      <c r="D107" s="156"/>
+      <c r="E107" s="157"/>
       <c r="F107"/>
     </row>
     <row r="108" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="61"/>
+      <c r="A108" s="55"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
       <c r="D108" s="6"/>
@@ -3760,9 +3873,9 @@
       <c r="F108"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="61"/>
-      <c r="B109" s="80" t="s">
-        <v>27</v>
+      <c r="A109" s="55"/>
+      <c r="B109" s="66" t="s">
+        <v>26</v>
       </c>
       <c r="C109" s="6"/>
       <c r="D109" s="6"/>
@@ -3770,21 +3883,21 @@
       <c r="F109"/>
     </row>
     <row r="110" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="62"/>
-      <c r="B110" s="63"/>
-      <c r="C110" s="63"/>
-      <c r="D110" s="63"/>
-      <c r="E110" s="64"/>
+      <c r="A110" s="56"/>
+      <c r="B110" s="57"/>
+      <c r="C110" s="57"/>
+      <c r="D110" s="57"/>
+      <c r="E110" s="58"/>
       <c r="F110"/>
     </row>
     <row r="111" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="65" t="s">
-        <v>13</v>
-      </c>
-      <c r="B111" s="66"/>
-      <c r="C111" s="66"/>
-      <c r="D111" s="66"/>
-      <c r="E111" s="67"/>
+      <c r="A111" s="155" t="s">
+        <v>12</v>
+      </c>
+      <c r="B111" s="156"/>
+      <c r="C111" s="156"/>
+      <c r="D111" s="156"/>
+      <c r="E111" s="157"/>
       <c r="F111"/>
     </row>
     <row r="112" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -3796,8 +3909,8 @@
       <c r="F112"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="83" t="s">
-        <v>26</v>
+      <c r="A113" s="69" t="s">
+        <v>25</v>
       </c>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -3822,13 +3935,13 @@
       <c r="F115"/>
     </row>
     <row r="116" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="65" t="s">
-        <v>15</v>
-      </c>
-      <c r="B116" s="66"/>
-      <c r="C116" s="66"/>
-      <c r="D116" s="66"/>
-      <c r="E116" s="67"/>
+      <c r="A116" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="B116" s="60"/>
+      <c r="C116" s="60"/>
+      <c r="D116" s="60"/>
+      <c r="E116" s="61"/>
       <c r="F116"/>
     </row>
     <row r="117" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -3841,8 +3954,8 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="8"/>
-      <c r="B118" s="80" t="s">
-        <v>44</v>
+      <c r="B118" s="66" t="s">
+        <v>41</v>
       </c>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
@@ -3866,9 +3979,9 @@
       <c r="F120"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="61"/>
-      <c r="B121" s="81" t="s">
-        <v>45</v>
+      <c r="A121" s="55"/>
+      <c r="B121" s="67" t="s">
+        <v>42</v>
       </c>
       <c r="C121" s="6"/>
       <c r="D121" s="6"/>
@@ -3876,26 +3989,26 @@
       <c r="F121"/>
     </row>
     <row r="122" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="62"/>
-      <c r="B122" s="63"/>
-      <c r="C122" s="63"/>
-      <c r="D122" s="63"/>
-      <c r="E122" s="64"/>
+      <c r="A122" s="56"/>
+      <c r="B122" s="57"/>
+      <c r="C122" s="57"/>
+      <c r="D122" s="57"/>
+      <c r="E122" s="58"/>
       <c r="F122"/>
     </row>
     <row r="123" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="B123" s="71"/>
-      <c r="C123" s="71"/>
-      <c r="D123" s="71"/>
-      <c r="E123" s="72"/>
+      <c r="A123" s="158" t="s">
+        <v>20</v>
+      </c>
+      <c r="B123" s="159"/>
+      <c r="C123" s="159"/>
+      <c r="D123" s="159"/>
+      <c r="E123" s="160"/>
       <c r="F123"/>
     </row>
     <row r="124" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A124" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -3904,40 +4017,40 @@
       <c r="F124"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="145"/>
-      <c r="B125" s="146"/>
-      <c r="C125" s="146"/>
-      <c r="D125" s="146"/>
-      <c r="E125" s="147"/>
+      <c r="A125" s="100"/>
+      <c r="B125" s="101"/>
+      <c r="C125" s="101"/>
+      <c r="D125" s="101"/>
+      <c r="E125" s="102"/>
       <c r="F125"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="145"/>
-      <c r="B126" s="146"/>
-      <c r="C126" s="146"/>
-      <c r="D126" s="146"/>
-      <c r="E126" s="147"/>
+      <c r="A126" s="100"/>
+      <c r="B126" s="101"/>
+      <c r="C126" s="101"/>
+      <c r="D126" s="101"/>
+      <c r="E126" s="102"/>
       <c r="F126"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="145"/>
-      <c r="B127" s="146"/>
-      <c r="C127" s="146"/>
-      <c r="D127" s="146"/>
-      <c r="E127" s="147"/>
+      <c r="A127" s="100"/>
+      <c r="B127" s="101"/>
+      <c r="C127" s="101"/>
+      <c r="D127" s="101"/>
+      <c r="E127" s="102"/>
       <c r="F127"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="145"/>
-      <c r="B128" s="146"/>
-      <c r="C128" s="146"/>
-      <c r="D128" s="146"/>
-      <c r="E128" s="147"/>
+      <c r="A128" s="100"/>
+      <c r="B128" s="101"/>
+      <c r="C128" s="101"/>
+      <c r="D128" s="101"/>
+      <c r="E128" s="102"/>
       <c r="F128"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -3946,71 +4059,71 @@
       <c r="F129"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" s="148"/>
-      <c r="B130" s="149"/>
-      <c r="C130" s="149"/>
-      <c r="D130" s="149"/>
-      <c r="E130" s="150"/>
+      <c r="A130" s="103"/>
+      <c r="B130" s="104"/>
+      <c r="C130" s="104"/>
+      <c r="D130" s="104"/>
+      <c r="E130" s="105"/>
       <c r="F130"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" s="148"/>
-      <c r="B131" s="149"/>
-      <c r="C131" s="149"/>
-      <c r="D131" s="149"/>
-      <c r="E131" s="150"/>
+      <c r="A131" s="103"/>
+      <c r="B131" s="104"/>
+      <c r="C131" s="104"/>
+      <c r="D131" s="104"/>
+      <c r="E131" s="105"/>
       <c r="F131"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" s="148"/>
-      <c r="B132" s="149"/>
-      <c r="C132" s="149"/>
-      <c r="D132" s="149"/>
-      <c r="E132" s="150"/>
+      <c r="A132" s="103"/>
+      <c r="B132" s="104"/>
+      <c r="C132" s="104"/>
+      <c r="D132" s="104"/>
+      <c r="E132" s="105"/>
       <c r="F132"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" s="148"/>
-      <c r="B133" s="149"/>
-      <c r="C133" s="149"/>
-      <c r="D133" s="149"/>
-      <c r="E133" s="150"/>
+      <c r="A133" s="103"/>
+      <c r="B133" s="104"/>
+      <c r="C133" s="104"/>
+      <c r="D133" s="104"/>
+      <c r="E133" s="105"/>
       <c r="F133"/>
     </row>
     <row r="134" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="151"/>
-      <c r="B134" s="152"/>
-      <c r="C134" s="152"/>
-      <c r="D134" s="152"/>
-      <c r="E134" s="153"/>
+      <c r="A134" s="106"/>
+      <c r="B134" s="107"/>
+      <c r="C134" s="107"/>
+      <c r="D134" s="107"/>
+      <c r="E134" s="108"/>
       <c r="F134"/>
     </row>
     <row r="135" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="74" t="s">
-        <v>22</v>
-      </c>
-      <c r="B135" s="71"/>
-      <c r="C135" s="71"/>
-      <c r="D135" s="71"/>
-      <c r="E135" s="72"/>
+      <c r="A135" s="158" t="s">
+        <v>21</v>
+      </c>
+      <c r="B135" s="159"/>
+      <c r="C135" s="159"/>
+      <c r="D135" s="159"/>
+      <c r="E135" s="160"/>
       <c r="F135"/>
     </row>
     <row r="136" spans="1:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="78" t="s">
-        <v>41</v>
-      </c>
-      <c r="B136" s="75"/>
-      <c r="C136" s="75"/>
-      <c r="D136" s="75"/>
-      <c r="E136" s="76"/>
+      <c r="A136" s="161" t="s">
+        <v>38</v>
+      </c>
+      <c r="B136" s="162"/>
+      <c r="C136" s="162"/>
+      <c r="D136" s="162"/>
+      <c r="E136" s="163"/>
       <c r="F136"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" s="94"/>
-      <c r="B137" s="95"/>
-      <c r="C137" s="95"/>
-      <c r="D137" s="95"/>
-      <c r="E137" s="96"/>
+      <c r="A137" s="80"/>
+      <c r="B137" s="81"/>
+      <c r="C137" s="81"/>
+      <c r="D137" s="81"/>
+      <c r="E137" s="82"/>
       <c r="F137"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -4058,8 +4171,8 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="8"/>
-      <c r="B144" s="79" t="s">
-        <v>23</v>
+      <c r="B144" s="65" t="s">
+        <v>22</v>
       </c>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
@@ -4082,7 +4195,23 @@
     <row r="147" spans="1:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="244" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="31">
+    <mergeCell ref="A135:E135"/>
+    <mergeCell ref="A136:E136"/>
+    <mergeCell ref="A100:E100"/>
+    <mergeCell ref="A73:E73"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="A125:E128"/>
     <mergeCell ref="A130:E134"/>
     <mergeCell ref="B12:E16"/>
@@ -4094,17 +4223,10 @@
     <mergeCell ref="C101:E101"/>
     <mergeCell ref="C102:E102"/>
     <mergeCell ref="C103:E103"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A111:E111"/>
+    <mergeCell ref="A107:E107"/>
+    <mergeCell ref="A123:E123"/>
+    <mergeCell ref="B23:E23"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.26" right="0.14000000000000001" top="0.4" bottom="0.11" header="0.23333333333333334" footer="0.5"/>

</xml_diff>